<commit_message>
new protocol commands: binPayload, cmd88
</commit_message>
<xml_diff>
--- a/doc/conversations/DVR conversation 24122022.xlsx
+++ b/doc/conversations/DVR conversation 24122022.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/den/brod-video/doc/conversations/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD0C7EA6-2C6A-9840-B432-5DF2C29B1C1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E0C4889-A8C0-5946-B585-D4A6B5E89F3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3420" yWindow="1000" windowWidth="25380" windowHeight="15600" xr2:uid="{975EE5A9-D02E-564E-A719-162CF0E3A1AF}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="820" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="825" uniqueCount="171">
   <si>
     <t>9.073099</t>
   </si>
@@ -305,12 +305,6 @@
     <t>Length</t>
   </si>
   <si>
-    <t>CmdID</t>
-  </si>
-  <si>
-    <t>ConnID</t>
-  </si>
-  <si>
     <t>49954 → 58452</t>
   </si>
   <si>
@@ -534,6 +528,27 @@
   </si>
   <si>
     <t>030000000020000006000000000000000000000000000000000000000018ae94124f0000000902010000000000000000000000000000000000000000</t>
+  </si>
+  <si>
+    <t>ConvID</t>
+  </si>
+  <si>
+    <t>Data1</t>
+  </si>
+  <si>
+    <t>Data2</t>
+  </si>
+  <si>
+    <t>Data3</t>
+  </si>
+  <si>
+    <t>Head</t>
+  </si>
+  <si>
+    <t>Tail</t>
+  </si>
+  <si>
+    <t>Data4</t>
   </si>
 </sst>
 </file>
@@ -564,7 +579,7 @@
       <family val="1"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -580,6 +595,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -605,7 +626,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -632,6 +653,16 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -949,7 +980,7 @@
   <dimension ref="A1:O82"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="G1" sqref="G1:M1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -981,17 +1012,27 @@
       <c r="F1" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="G1" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1"/>
-      <c r="L1" s="1"/>
-      <c r="M1" s="1"/>
+      <c r="G1" s="15" t="s">
+        <v>168</v>
+      </c>
+      <c r="H1" s="15" t="s">
+        <v>164</v>
+      </c>
+      <c r="I1" s="15" t="s">
+        <v>165</v>
+      </c>
+      <c r="J1" s="15" t="s">
+        <v>166</v>
+      </c>
+      <c r="K1" s="15" t="s">
+        <v>167</v>
+      </c>
+      <c r="L1" s="15" t="s">
+        <v>170</v>
+      </c>
+      <c r="M1" s="15" t="s">
+        <v>169</v>
+      </c>
       <c r="N1" s="1"/>
       <c r="O1" s="1"/>
     </row>
@@ -1009,16 +1050,16 @@
         <v>2</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="G2" s="7">
         <v>1000100</v>
       </c>
       <c r="H2" s="7" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="I2" s="7">
         <v>0</v>
@@ -1027,13 +1068,13 @@
         <v>0</v>
       </c>
       <c r="K2" s="7" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="L2" s="7">
         <v>0</v>
       </c>
       <c r="M2" s="7" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.2">
@@ -1050,16 +1091,16 @@
         <v>1</v>
       </c>
       <c r="E3" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="F3" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="G3" s="4">
         <v>1000100</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="I3" s="4">
         <v>0</v>
@@ -1068,13 +1109,13 @@
         <v>0</v>
       </c>
       <c r="K3" s="4" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="L3" s="4">
         <v>0</v>
       </c>
       <c r="M3" s="4" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.2">
@@ -1091,31 +1132,31 @@
         <v>2</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="G4" s="7">
         <v>1000100</v>
       </c>
       <c r="H4" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="I4" s="7" t="s">
         <v>115</v>
       </c>
-      <c r="I4" s="7" t="s">
-        <v>117</v>
-      </c>
       <c r="J4" s="7">
         <v>0</v>
       </c>
       <c r="K4" s="7" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="L4" s="7" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="M4" s="7" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.2">
@@ -1132,31 +1173,31 @@
         <v>1</v>
       </c>
       <c r="E5" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="F5" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="G5" s="4">
         <v>1000100</v>
       </c>
       <c r="H5" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="I5" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="I5" s="4" t="s">
-        <v>117</v>
-      </c>
       <c r="J5" s="4">
         <v>0</v>
       </c>
       <c r="K5" s="4" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="L5" s="4" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="M5" s="4" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.2">
@@ -1173,31 +1214,31 @@
         <v>2</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="G6" s="7">
         <v>1000100</v>
       </c>
       <c r="H6" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="I6" s="7" t="s">
         <v>115</v>
       </c>
-      <c r="I6" s="7" t="s">
-        <v>117</v>
-      </c>
       <c r="J6" s="7" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="K6" s="7" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="L6" s="7" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="M6" s="7" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.2">
@@ -1214,31 +1255,31 @@
         <v>1</v>
       </c>
       <c r="E7" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="F7" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="G7" s="4">
         <v>1000100</v>
       </c>
       <c r="H7" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="I7" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="I7" s="4" t="s">
-        <v>117</v>
-      </c>
       <c r="J7" s="4" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="K7" s="4" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="L7" s="4" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="M7" s="4" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.2">
@@ -1255,74 +1296,74 @@
         <v>1</v>
       </c>
       <c r="E8" s="8" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="F8" s="8" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="G8" s="10">
         <v>1010100</v>
       </c>
       <c r="H8" s="10" t="s">
+        <v>113</v>
+      </c>
+      <c r="I8" s="10" t="s">
+        <v>113</v>
+      </c>
+      <c r="J8" s="10" t="s">
         <v>115</v>
       </c>
-      <c r="I8" s="10" t="s">
-        <v>115</v>
-      </c>
-      <c r="J8" s="10" t="s">
-        <v>117</v>
-      </c>
       <c r="K8" s="10" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="L8" s="10" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="M8" s="10">
         <v>68656164</v>
       </c>
       <c r="N8" s="11" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A9">
+      <c r="A9" s="12">
         <v>2508</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B9" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="C9" t="s">
-        <v>1</v>
-      </c>
-      <c r="D9" t="s">
-        <v>2</v>
-      </c>
-      <c r="E9" t="s">
-        <v>91</v>
-      </c>
-      <c r="F9" t="s">
-        <v>95</v>
-      </c>
-      <c r="G9" s="4">
+      <c r="C9" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="D9" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="E9" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="F9" s="12" t="s">
+        <v>93</v>
+      </c>
+      <c r="G9" s="14">
         <v>1020100</v>
       </c>
-      <c r="H9" s="4" t="s">
+      <c r="H9" s="14" t="s">
+        <v>113</v>
+      </c>
+      <c r="I9" s="14" t="s">
         <v>115</v>
       </c>
-      <c r="I9" s="4" t="s">
-        <v>117</v>
-      </c>
-      <c r="J9" s="4" t="s">
-        <v>115</v>
-      </c>
-      <c r="K9" s="4">
-        <v>0</v>
-      </c>
-      <c r="L9" s="4" t="s">
-        <v>118</v>
-      </c>
-      <c r="M9" s="4"/>
+      <c r="J9" s="14" t="s">
+        <v>113</v>
+      </c>
+      <c r="K9" s="14">
+        <v>0</v>
+      </c>
+      <c r="L9" s="14" t="s">
+        <v>116</v>
+      </c>
+      <c r="M9" s="14"/>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A10">
@@ -1338,34 +1379,34 @@
         <v>2</v>
       </c>
       <c r="E10" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="F10" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="G10" s="4">
         <v>1010100</v>
       </c>
       <c r="H10" s="4" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="I10" s="4" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="J10" s="4" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="K10" s="4" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="L10" s="4" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="M10" s="4">
         <v>31313131</v>
       </c>
       <c r="N10" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.2">
@@ -1382,28 +1423,28 @@
         <v>1</v>
       </c>
       <c r="E11" t="s">
+        <v>91</v>
+      </c>
+      <c r="F11" t="s">
         <v>93</v>
-      </c>
-      <c r="F11" t="s">
-        <v>95</v>
       </c>
       <c r="G11" s="4">
         <v>1020100</v>
       </c>
       <c r="H11" s="4" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="I11" s="4" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="J11" s="4" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="K11" s="4">
         <v>0</v>
       </c>
       <c r="L11" s="4" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="M11" s="4"/>
     </row>
@@ -1421,34 +1462,34 @@
         <v>1</v>
       </c>
       <c r="E12" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="F12" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="G12" s="4">
         <v>1010100</v>
       </c>
       <c r="H12" s="4" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="I12" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="J12" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="K12" s="4" t="s">
         <v>118</v>
       </c>
-      <c r="J12" s="4" t="s">
-        <v>115</v>
-      </c>
-      <c r="K12" s="4" t="s">
-        <v>120</v>
-      </c>
       <c r="L12" s="4" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="M12" s="4">
         <v>31313131</v>
       </c>
       <c r="N12" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.2">
@@ -1465,34 +1506,34 @@
         <v>1</v>
       </c>
       <c r="E13" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="F13" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="G13" s="4">
         <v>1010100</v>
       </c>
       <c r="H13" s="4" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="I13" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="J13" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="K13" s="4" t="s">
         <v>120</v>
       </c>
-      <c r="J13" s="4" t="s">
-        <v>115</v>
-      </c>
-      <c r="K13" s="4" t="s">
-        <v>122</v>
-      </c>
       <c r="L13" s="4" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="M13" s="4">
         <v>0</v>
       </c>
       <c r="N13" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.2">
@@ -1509,28 +1550,28 @@
         <v>2</v>
       </c>
       <c r="E14" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="F14" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="G14" s="4">
         <v>1020100</v>
       </c>
       <c r="H14" s="4" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="I14" s="4" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="J14" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="K14" s="4">
+        <v>0</v>
+      </c>
+      <c r="L14" s="4" t="s">
         <v>118</v>
-      </c>
-      <c r="K14" s="4">
-        <v>0</v>
-      </c>
-      <c r="L14" s="4" t="s">
-        <v>120</v>
       </c>
       <c r="M14" s="4"/>
     </row>
@@ -1548,28 +1589,28 @@
         <v>2</v>
       </c>
       <c r="E15" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="F15" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="G15" s="4">
         <v>1020100</v>
       </c>
       <c r="H15" s="4" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="I15" s="4" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="J15" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="K15" s="4">
+        <v>0</v>
+      </c>
+      <c r="L15" s="4" t="s">
         <v>120</v>
-      </c>
-      <c r="K15" s="4">
-        <v>0</v>
-      </c>
-      <c r="L15" s="4" t="s">
-        <v>122</v>
       </c>
       <c r="M15" s="4"/>
     </row>
@@ -1587,34 +1628,34 @@
         <v>2</v>
       </c>
       <c r="E16" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="F16" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="G16" s="4">
         <v>1010100</v>
       </c>
       <c r="H16" s="4" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="I16" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="J16" s="4" t="s">
         <v>118</v>
       </c>
-      <c r="J16" s="4" t="s">
+      <c r="K16" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="L16" s="4" t="s">
         <v>120</v>
-      </c>
-      <c r="K16" s="4" t="s">
-        <v>120</v>
-      </c>
-      <c r="L16" s="4" t="s">
-        <v>122</v>
       </c>
       <c r="M16" s="4">
         <v>31313131</v>
       </c>
       <c r="N16" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.2">
@@ -1631,28 +1672,28 @@
         <v>1</v>
       </c>
       <c r="E17" t="s">
+        <v>91</v>
+      </c>
+      <c r="F17" t="s">
         <v>93</v>
-      </c>
-      <c r="F17" t="s">
-        <v>95</v>
       </c>
       <c r="G17" s="4">
         <v>1020100</v>
       </c>
       <c r="H17" s="4" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="I17" s="4" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="J17" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="K17" s="4">
+        <v>0</v>
+      </c>
+      <c r="L17" s="4" t="s">
         <v>118</v>
-      </c>
-      <c r="K17" s="4">
-        <v>0</v>
-      </c>
-      <c r="L17" s="4" t="s">
-        <v>120</v>
       </c>
       <c r="M17" s="4"/>
     </row>
@@ -1670,34 +1711,34 @@
         <v>1</v>
       </c>
       <c r="E18" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="F18" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="G18" s="4">
         <v>1010100</v>
       </c>
       <c r="H18" s="4" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="I18" s="4" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="J18" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="K18" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="L18" s="4" t="s">
         <v>118</v>
-      </c>
-      <c r="K18" s="4" t="s">
-        <v>125</v>
-      </c>
-      <c r="L18" s="4" t="s">
-        <v>120</v>
       </c>
       <c r="M18" s="4">
         <v>31313131</v>
       </c>
       <c r="N18" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.2">
@@ -1714,34 +1755,34 @@
         <v>1</v>
       </c>
       <c r="E19" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="F19" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="G19" s="4">
         <v>1010100</v>
       </c>
       <c r="H19" s="4" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="I19" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="J19" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="K19" s="4" t="s">
         <v>125</v>
       </c>
-      <c r="J19" s="4" t="s">
+      <c r="L19" s="4" t="s">
         <v>118</v>
       </c>
-      <c r="K19" s="4" t="s">
+      <c r="M19" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="N19" t="s">
         <v>127</v>
-      </c>
-      <c r="L19" s="4" t="s">
-        <v>120</v>
-      </c>
-      <c r="M19" s="4" t="s">
-        <v>128</v>
-      </c>
-      <c r="N19" t="s">
-        <v>129</v>
       </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.2">
@@ -1758,28 +1799,28 @@
         <v>2</v>
       </c>
       <c r="E20" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="F20" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="G20" s="4">
         <v>1020100</v>
       </c>
       <c r="H20" s="4" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="I20" s="4" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="J20" s="4" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="K20" s="4">
         <v>0</v>
       </c>
       <c r="L20" s="4" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="M20" s="4"/>
     </row>
@@ -1797,28 +1838,28 @@
         <v>2</v>
       </c>
       <c r="E21" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="F21" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="G21" s="4">
         <v>1020100</v>
       </c>
       <c r="H21" s="4" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="I21" s="4" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="J21" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="K21" s="4">
+        <v>0</v>
+      </c>
+      <c r="L21" s="4" t="s">
         <v>125</v>
-      </c>
-      <c r="K21" s="4">
-        <v>0</v>
-      </c>
-      <c r="L21" s="4" t="s">
-        <v>127</v>
       </c>
       <c r="M21" s="4"/>
     </row>
@@ -1836,34 +1877,34 @@
         <v>2</v>
       </c>
       <c r="E22" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="F22" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="G22" s="4">
         <v>1010100</v>
       </c>
       <c r="H22" s="4" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="I22" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="J22" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="K22" s="4" t="s">
         <v>120</v>
       </c>
-      <c r="J22" s="4" t="s">
+      <c r="L22" s="4" t="s">
         <v>125</v>
-      </c>
-      <c r="K22" s="4" t="s">
-        <v>122</v>
-      </c>
-      <c r="L22" s="4" t="s">
-        <v>127</v>
       </c>
       <c r="M22" s="4">
         <v>31313131</v>
       </c>
       <c r="N22" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.2">
@@ -1880,34 +1921,34 @@
         <v>2</v>
       </c>
       <c r="E23" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="F23" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="G23" s="4">
         <v>1010100</v>
       </c>
       <c r="H23" s="4" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="I23" s="4" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="J23" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="K23" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="L23" s="4" t="s">
         <v>125</v>
-      </c>
-      <c r="K23" s="4" t="s">
-        <v>125</v>
-      </c>
-      <c r="L23" s="4" t="s">
-        <v>127</v>
       </c>
       <c r="M23" s="4">
         <v>31313131</v>
       </c>
       <c r="N23" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.2">
@@ -1924,34 +1965,34 @@
         <v>2</v>
       </c>
       <c r="E24" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="F24" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="G24" s="4">
         <v>1010100</v>
       </c>
       <c r="H24" s="4" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="I24" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="J24" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="K24" s="4" t="s">
         <v>125</v>
       </c>
-      <c r="J24" s="4" t="s">
+      <c r="L24" s="4" t="s">
         <v>125</v>
-      </c>
-      <c r="K24" s="4" t="s">
-        <v>127</v>
-      </c>
-      <c r="L24" s="4" t="s">
-        <v>127</v>
       </c>
       <c r="M24" s="4">
         <v>31313131</v>
       </c>
       <c r="N24" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.2">
@@ -1968,34 +2009,34 @@
         <v>2</v>
       </c>
       <c r="E25" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="F25" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="G25" s="4">
         <v>1010100</v>
       </c>
       <c r="H25" s="4" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="I25" s="4" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="J25" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="K25" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="L25" s="4" t="s">
         <v>125</v>
-      </c>
-      <c r="K25" s="4" t="s">
-        <v>132</v>
-      </c>
-      <c r="L25" s="4" t="s">
-        <v>127</v>
       </c>
       <c r="M25" s="4">
         <v>31313131</v>
       </c>
       <c r="N25" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.2">
@@ -2012,34 +2053,34 @@
         <v>2</v>
       </c>
       <c r="E26" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="F26" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="G26" s="4">
         <v>1010100</v>
       </c>
       <c r="H26" s="4" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="I26" s="4" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="J26" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="K26" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="L26" s="4" t="s">
         <v>125</v>
-      </c>
-      <c r="K26" s="4" t="s">
-        <v>133</v>
-      </c>
-      <c r="L26" s="4" t="s">
-        <v>127</v>
       </c>
       <c r="M26" s="4">
         <v>31313131</v>
       </c>
       <c r="N26" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.2">
@@ -2056,34 +2097,34 @@
         <v>2</v>
       </c>
       <c r="E27" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="F27" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="G27" s="4">
         <v>1010100</v>
       </c>
       <c r="H27" s="4" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="I27" s="4" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="J27" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="K27" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="L27" s="4" t="s">
         <v>125</v>
-      </c>
-      <c r="K27" s="4" t="s">
-        <v>134</v>
-      </c>
-      <c r="L27" s="4" t="s">
-        <v>127</v>
       </c>
       <c r="M27" s="4">
         <v>31313131</v>
       </c>
       <c r="N27" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.2">
@@ -2100,34 +2141,34 @@
         <v>2</v>
       </c>
       <c r="E28" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="F28" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="G28" s="4">
         <v>1010100</v>
       </c>
       <c r="H28" s="4" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="I28" s="4" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="J28" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="K28" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="L28" s="4" t="s">
         <v>125</v>
-      </c>
-      <c r="K28" s="4" t="s">
-        <v>135</v>
-      </c>
-      <c r="L28" s="4" t="s">
-        <v>127</v>
       </c>
       <c r="M28" s="4">
         <v>31313131</v>
       </c>
       <c r="N28" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.2">
@@ -2144,34 +2185,34 @@
         <v>2</v>
       </c>
       <c r="E29" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="F29" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="G29" s="4">
         <v>1010100</v>
       </c>
       <c r="H29" s="4" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="I29" s="4" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="J29" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="K29" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="L29" s="4" t="s">
         <v>125</v>
-      </c>
-      <c r="K29" s="4" t="s">
-        <v>136</v>
-      </c>
-      <c r="L29" s="4" t="s">
-        <v>127</v>
       </c>
       <c r="M29" s="4">
         <v>31313131</v>
       </c>
       <c r="N29" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.2">
@@ -2188,34 +2229,34 @@
         <v>2</v>
       </c>
       <c r="E30" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="F30" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="G30" s="4">
         <v>1010100</v>
       </c>
       <c r="H30" s="4" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="I30" s="4" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="J30" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="K30" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="L30" s="4" t="s">
         <v>125</v>
-      </c>
-      <c r="K30" s="4" t="s">
-        <v>137</v>
-      </c>
-      <c r="L30" s="4" t="s">
-        <v>127</v>
       </c>
       <c r="M30" s="4">
         <v>31313131</v>
       </c>
       <c r="N30" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.2">
@@ -2232,34 +2273,34 @@
         <v>2</v>
       </c>
       <c r="E31" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="F31" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="G31" s="4">
         <v>1010100</v>
       </c>
       <c r="H31" s="4" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="I31" s="4" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="J31" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="K31" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="L31" s="4" t="s">
         <v>125</v>
-      </c>
-      <c r="K31" s="4" t="s">
-        <v>138</v>
-      </c>
-      <c r="L31" s="4" t="s">
-        <v>127</v>
       </c>
       <c r="M31" s="4">
         <v>31313131</v>
       </c>
       <c r="N31" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.2">
@@ -2276,28 +2317,28 @@
         <v>2</v>
       </c>
       <c r="E32" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="F32" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="G32" s="4">
         <v>1010100</v>
       </c>
       <c r="H32" s="4" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="I32" s="4" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="J32" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="K32" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="L32" s="4" t="s">
         <v>125</v>
-      </c>
-      <c r="K32" s="4" t="s">
-        <v>139</v>
-      </c>
-      <c r="L32" s="4" t="s">
-        <v>127</v>
       </c>
       <c r="M32" s="4">
         <v>31313131</v>
@@ -2320,28 +2361,28 @@
         <v>1</v>
       </c>
       <c r="E33" t="s">
+        <v>91</v>
+      </c>
+      <c r="F33" t="s">
         <v>93</v>
-      </c>
-      <c r="F33" t="s">
-        <v>95</v>
       </c>
       <c r="G33" s="4">
         <v>1020100</v>
       </c>
       <c r="H33" s="4" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="I33" s="4" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="J33" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="K33" s="4">
+        <v>0</v>
+      </c>
+      <c r="L33" s="4" t="s">
         <v>120</v>
-      </c>
-      <c r="K33" s="4">
-        <v>0</v>
-      </c>
-      <c r="L33" s="4" t="s">
-        <v>122</v>
       </c>
       <c r="M33" s="4"/>
     </row>
@@ -2359,28 +2400,28 @@
         <v>1</v>
       </c>
       <c r="E34" t="s">
+        <v>91</v>
+      </c>
+      <c r="F34" t="s">
         <v>93</v>
-      </c>
-      <c r="F34" t="s">
-        <v>95</v>
       </c>
       <c r="G34" s="4">
         <v>1020100</v>
       </c>
       <c r="H34" s="4" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="I34" s="4" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="J34" s="4" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="K34" s="4">
         <v>0</v>
       </c>
       <c r="L34" s="4" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="M34" s="4"/>
     </row>
@@ -2398,28 +2439,28 @@
         <v>1</v>
       </c>
       <c r="E35" t="s">
+        <v>91</v>
+      </c>
+      <c r="F35" t="s">
         <v>93</v>
-      </c>
-      <c r="F35" t="s">
-        <v>95</v>
       </c>
       <c r="G35" s="4">
         <v>1020100</v>
       </c>
       <c r="H35" s="4" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="I35" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="J35" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="K35" s="4">
+        <v>0</v>
+      </c>
+      <c r="L35" s="4" t="s">
         <v>125</v>
-      </c>
-      <c r="J35" s="4" t="s">
-        <v>125</v>
-      </c>
-      <c r="K35" s="4">
-        <v>0</v>
-      </c>
-      <c r="L35" s="4" t="s">
-        <v>127</v>
       </c>
       <c r="M35" s="4"/>
     </row>
@@ -2437,34 +2478,34 @@
         <v>1</v>
       </c>
       <c r="E36" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="F36" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="G36" s="4">
         <v>1010100</v>
       </c>
       <c r="H36" s="4" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="I36" s="4" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="J36" s="4" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="K36" s="4" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="L36" s="4" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="M36" s="4">
         <v>31313131</v>
       </c>
       <c r="N36" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.2">
@@ -2481,28 +2522,28 @@
         <v>1</v>
       </c>
       <c r="E37" t="s">
+        <v>91</v>
+      </c>
+      <c r="F37" t="s">
         <v>93</v>
-      </c>
-      <c r="F37" t="s">
-        <v>95</v>
       </c>
       <c r="G37" s="4">
         <v>1020100</v>
       </c>
       <c r="H37" s="4" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="I37" s="4" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="J37" s="4" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="K37" s="4">
         <v>0</v>
       </c>
       <c r="L37" s="4" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="M37" s="4"/>
     </row>
@@ -2520,28 +2561,28 @@
         <v>2</v>
       </c>
       <c r="E38" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="F38" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="G38" s="4">
         <v>1020100</v>
       </c>
       <c r="H38" s="4" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="I38" s="4" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="J38" s="4" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="K38" s="4">
         <v>0</v>
       </c>
       <c r="L38" s="4" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="M38" s="4"/>
     </row>
@@ -2559,28 +2600,28 @@
         <v>1</v>
       </c>
       <c r="E39" t="s">
+        <v>91</v>
+      </c>
+      <c r="F39" t="s">
         <v>93</v>
-      </c>
-      <c r="F39" t="s">
-        <v>95</v>
       </c>
       <c r="G39" s="4">
         <v>1020100</v>
       </c>
       <c r="H39" s="4" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="I39" s="4" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="J39" s="4" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="K39" s="4">
         <v>0</v>
       </c>
       <c r="L39" s="4" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="M39" s="4"/>
     </row>
@@ -2598,28 +2639,28 @@
         <v>1</v>
       </c>
       <c r="E40" t="s">
+        <v>91</v>
+      </c>
+      <c r="F40" t="s">
         <v>93</v>
-      </c>
-      <c r="F40" t="s">
-        <v>95</v>
       </c>
       <c r="G40" s="4">
         <v>1020100</v>
       </c>
       <c r="H40" s="4" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="I40" s="4" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="J40" s="4" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="K40" s="4">
         <v>0</v>
       </c>
       <c r="L40" s="4" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="M40" s="4"/>
     </row>
@@ -2637,28 +2678,28 @@
         <v>1</v>
       </c>
       <c r="E41" t="s">
+        <v>91</v>
+      </c>
+      <c r="F41" t="s">
         <v>93</v>
-      </c>
-      <c r="F41" t="s">
-        <v>95</v>
       </c>
       <c r="G41" s="4">
         <v>1020100</v>
       </c>
       <c r="H41" s="4" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="I41" s="4" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="J41" s="4" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="K41" s="4">
         <v>0</v>
       </c>
       <c r="L41" s="4" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="M41" s="4"/>
     </row>
@@ -2676,28 +2717,28 @@
         <v>1</v>
       </c>
       <c r="E42" t="s">
+        <v>91</v>
+      </c>
+      <c r="F42" t="s">
         <v>93</v>
-      </c>
-      <c r="F42" t="s">
-        <v>95</v>
       </c>
       <c r="G42" s="4">
         <v>1020100</v>
       </c>
       <c r="H42" s="4" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="I42" s="4" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="J42" s="4" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="K42" s="4">
         <v>0</v>
       </c>
       <c r="L42" s="4" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="M42" s="4"/>
     </row>
@@ -2715,28 +2756,28 @@
         <v>1</v>
       </c>
       <c r="E43" t="s">
+        <v>91</v>
+      </c>
+      <c r="F43" t="s">
         <v>93</v>
-      </c>
-      <c r="F43" t="s">
-        <v>95</v>
       </c>
       <c r="G43" s="4">
         <v>1020100</v>
       </c>
       <c r="H43" s="4" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="I43" s="4" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="J43" s="4" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="K43" s="4">
         <v>0</v>
       </c>
       <c r="L43" s="4" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="M43" s="4"/>
     </row>
@@ -2754,28 +2795,28 @@
         <v>1</v>
       </c>
       <c r="E44" t="s">
+        <v>91</v>
+      </c>
+      <c r="F44" t="s">
         <v>93</v>
-      </c>
-      <c r="F44" t="s">
-        <v>95</v>
       </c>
       <c r="G44" s="4">
         <v>1020100</v>
       </c>
       <c r="H44" s="4" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="I44" s="4" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="J44" s="4" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="K44" s="4">
         <v>0</v>
       </c>
       <c r="L44" s="4" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="M44" s="4"/>
     </row>
@@ -2793,34 +2834,34 @@
         <v>1</v>
       </c>
       <c r="E45" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="F45" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="G45" s="4">
         <v>1010100</v>
       </c>
       <c r="H45" s="4" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="I45" s="4" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="J45" s="4" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="K45" s="4" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="L45" s="4" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="M45" s="4">
         <v>31313131</v>
       </c>
       <c r="N45" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="46" spans="1:14" x14ac:dyDescent="0.2">
@@ -2837,34 +2878,34 @@
         <v>1</v>
       </c>
       <c r="E46" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="F46" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="G46" s="4">
         <v>1010100</v>
       </c>
       <c r="H46" s="4" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="I46" s="4" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="J46" s="4" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="K46" s="4" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="L46" s="4" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="M46" s="4">
         <v>0</v>
       </c>
       <c r="N46" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="47" spans="1:14" x14ac:dyDescent="0.2">
@@ -2881,34 +2922,34 @@
         <v>1</v>
       </c>
       <c r="E47" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="F47" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="G47" s="4">
         <v>1010100</v>
       </c>
       <c r="H47" s="4" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="I47" s="4" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="J47" s="4" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="K47" s="4" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="L47" s="4" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="M47" s="4">
         <v>0</v>
       </c>
       <c r="N47" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="48" spans="1:14" x14ac:dyDescent="0.2">
@@ -2925,28 +2966,28 @@
         <v>2</v>
       </c>
       <c r="E48" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="F48" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="G48" s="4">
         <v>1020100</v>
       </c>
       <c r="H48" s="4" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="I48" s="4" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="J48" s="4" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="K48" s="4">
         <v>0</v>
       </c>
       <c r="L48" s="4" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="M48" s="4"/>
     </row>
@@ -2964,28 +3005,28 @@
         <v>2</v>
       </c>
       <c r="E49" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="F49" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="G49" s="4">
         <v>1020100</v>
       </c>
       <c r="H49" s="4" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="I49" s="4" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="J49" s="4" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="K49" s="4">
         <v>0</v>
       </c>
       <c r="L49" s="4" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="M49" s="4"/>
     </row>
@@ -3003,28 +3044,28 @@
         <v>2</v>
       </c>
       <c r="E50" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="F50" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="G50" s="4">
         <v>1020100</v>
       </c>
       <c r="H50" s="4" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="I50" s="4" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="J50" s="4" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="K50" s="4">
         <v>0</v>
       </c>
       <c r="L50" s="4" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="M50" s="4"/>
     </row>
@@ -3042,34 +3083,34 @@
         <v>1</v>
       </c>
       <c r="E51" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="F51" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="G51" s="4">
         <v>1010100</v>
       </c>
       <c r="H51" s="4" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="I51" s="4" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="J51" s="4" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="K51" s="4" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="L51" s="4" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="M51" s="4">
         <v>31313131</v>
       </c>
       <c r="N51" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="52" spans="1:14" x14ac:dyDescent="0.2">
@@ -3086,28 +3127,28 @@
         <v>2</v>
       </c>
       <c r="E52" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="F52" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="G52" s="4">
         <v>1020100</v>
       </c>
       <c r="H52" s="4" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="I52" s="4" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="J52" s="4" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="K52" s="4">
         <v>0</v>
       </c>
       <c r="L52" s="4" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="M52" s="4"/>
     </row>
@@ -3125,34 +3166,34 @@
         <v>2</v>
       </c>
       <c r="E53" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="F53" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="G53" s="4">
         <v>1010100</v>
       </c>
       <c r="H53" s="4" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="I53" s="4" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="J53" s="4" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="K53" s="4" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="L53" s="4" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="M53" s="4">
         <v>31313131</v>
       </c>
       <c r="N53" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="54" spans="1:14" x14ac:dyDescent="0.2">
@@ -3169,34 +3210,34 @@
         <v>1</v>
       </c>
       <c r="E54" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="F54" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="G54" s="4">
         <v>1010100</v>
       </c>
       <c r="H54" s="4" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="I54" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="J54" s="4" t="s">
         <v>136</v>
       </c>
-      <c r="J54" s="4" t="s">
-        <v>138</v>
-      </c>
       <c r="K54" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="L54" s="4" t="s">
         <v>137</v>
-      </c>
-      <c r="L54" s="4" t="s">
-        <v>139</v>
       </c>
       <c r="M54" s="4">
         <v>31313131</v>
       </c>
       <c r="N54" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="55" spans="1:14" x14ac:dyDescent="0.2">
@@ -3213,28 +3254,28 @@
         <v>2</v>
       </c>
       <c r="E55" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="F55" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="G55" s="4">
         <v>1020100</v>
       </c>
       <c r="H55" s="4" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="I55" s="4" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="J55" s="4" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="K55" s="4">
         <v>0</v>
       </c>
       <c r="L55" s="4" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="M55" s="4"/>
     </row>
@@ -3252,34 +3293,34 @@
         <v>1</v>
       </c>
       <c r="E56" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="F56" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="G56" s="4">
         <v>1010100</v>
       </c>
       <c r="H56" s="4" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="I56" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="J56" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="K56" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="L56" s="4" t="s">
         <v>137</v>
       </c>
-      <c r="J56" s="4" t="s">
-        <v>138</v>
-      </c>
-      <c r="K56" s="4" t="s">
-        <v>138</v>
-      </c>
-      <c r="L56" s="4" t="s">
-        <v>139</v>
-      </c>
       <c r="M56" s="4" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="N56" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="57" spans="1:14" x14ac:dyDescent="0.2">
@@ -3296,28 +3337,28 @@
         <v>2</v>
       </c>
       <c r="E57" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="F57" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="G57" s="4">
         <v>1020100</v>
       </c>
       <c r="H57" s="4" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="I57" s="4" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="J57" s="4" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="K57" s="4">
         <v>0</v>
       </c>
       <c r="L57" s="4" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="M57" s="4"/>
     </row>
@@ -3335,28 +3376,28 @@
         <v>1</v>
       </c>
       <c r="E58" t="s">
+        <v>91</v>
+      </c>
+      <c r="F58" t="s">
         <v>93</v>
-      </c>
-      <c r="F58" t="s">
-        <v>95</v>
       </c>
       <c r="G58" s="4">
         <v>1020100</v>
       </c>
       <c r="H58" s="4" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="I58" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="J58" s="4" t="s">
         <v>137</v>
       </c>
-      <c r="J58" s="4" t="s">
-        <v>139</v>
-      </c>
       <c r="K58" s="4">
         <v>0</v>
       </c>
       <c r="L58" s="4" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="M58" s="4"/>
     </row>
@@ -3374,28 +3415,28 @@
         <v>1</v>
       </c>
       <c r="E59" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="F59" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="G59" s="4">
         <v>1010100</v>
       </c>
       <c r="H59" s="4" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="I59" s="4" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="J59" s="4" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="K59" s="4" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="L59" s="4" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="M59" s="4">
         <v>31313131</v>
@@ -3418,28 +3459,28 @@
         <v>2</v>
       </c>
       <c r="E60" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="F60" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="G60" s="4">
         <v>1020100</v>
       </c>
       <c r="H60" s="4" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="I60" s="4" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="J60" s="4" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="K60" s="4">
         <v>0</v>
       </c>
       <c r="L60" s="4" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="M60" s="4"/>
     </row>
@@ -3457,34 +3498,34 @@
         <v>1</v>
       </c>
       <c r="E61" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="F61" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="G61" s="4">
         <v>1010100</v>
       </c>
       <c r="H61" s="4" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="I61" s="4" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="J61" s="4" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="K61" s="4" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="L61" s="4" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="M61" s="4">
         <v>31313131</v>
       </c>
       <c r="N61" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="62" spans="1:14" x14ac:dyDescent="0.2">
@@ -3501,28 +3542,28 @@
         <v>2</v>
       </c>
       <c r="E62" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="F62" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="G62" s="4">
         <v>1020100</v>
       </c>
       <c r="H62" s="4" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="I62" s="4" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="J62" s="4" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="K62" s="4">
         <v>0</v>
       </c>
       <c r="L62" s="4" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="M62" s="4"/>
     </row>
@@ -3540,34 +3581,34 @@
         <v>1</v>
       </c>
       <c r="E63" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="F63" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="G63" s="4">
         <v>1010100</v>
       </c>
       <c r="H63" s="4" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="I63" s="4" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="J63" s="4" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="K63" s="4" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="L63" s="4" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="M63" s="4">
         <v>31313131</v>
       </c>
       <c r="N63" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="64" spans="1:14" x14ac:dyDescent="0.2">
@@ -3584,34 +3625,34 @@
         <v>1</v>
       </c>
       <c r="E64" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="F64" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="G64" s="4">
         <v>1010100</v>
       </c>
       <c r="H64" s="4" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="I64" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="J64" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="K64" s="4" t="s">
         <v>148</v>
       </c>
-      <c r="J64" s="4" t="s">
-        <v>139</v>
-      </c>
-      <c r="K64" s="4" t="s">
+      <c r="L64" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="M64" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="N64" t="s">
         <v>150</v>
-      </c>
-      <c r="L64" s="4" t="s">
-        <v>142</v>
-      </c>
-      <c r="M64" s="4" t="s">
-        <v>151</v>
-      </c>
-      <c r="N64" t="s">
-        <v>152</v>
       </c>
     </row>
     <row r="65" spans="1:14" x14ac:dyDescent="0.2">
@@ -3628,28 +3669,28 @@
         <v>2</v>
       </c>
       <c r="E65" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="F65" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="G65" s="4">
         <v>1020100</v>
       </c>
       <c r="H65" s="4" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="I65" s="4" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="J65" s="4" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="K65" s="4">
         <v>0</v>
       </c>
       <c r="L65" s="4" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="M65" s="4"/>
     </row>
@@ -3667,28 +3708,28 @@
         <v>2</v>
       </c>
       <c r="E66" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="F66" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="G66" s="4">
         <v>1020100</v>
       </c>
       <c r="H66" s="4" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="I66" s="4" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="J66" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="K66" s="4">
+        <v>0</v>
+      </c>
+      <c r="L66" s="4" t="s">
         <v>148</v>
-      </c>
-      <c r="K66" s="4">
-        <v>0</v>
-      </c>
-      <c r="L66" s="4" t="s">
-        <v>150</v>
       </c>
       <c r="M66" s="4"/>
     </row>
@@ -3706,34 +3747,34 @@
         <v>2</v>
       </c>
       <c r="E67" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="F67" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="G67" s="4">
         <v>1010100</v>
       </c>
       <c r="H67" s="4" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="I67" s="4" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="J67" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="K67" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="L67" s="4" t="s">
         <v>148</v>
-      </c>
-      <c r="K67" s="4" t="s">
-        <v>148</v>
-      </c>
-      <c r="L67" s="4" t="s">
-        <v>150</v>
       </c>
       <c r="M67" s="4">
         <v>31313131</v>
       </c>
       <c r="N67" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="68" spans="1:14" x14ac:dyDescent="0.2">
@@ -3750,34 +3791,34 @@
         <v>2</v>
       </c>
       <c r="E68" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="F68" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="G68" s="4">
         <v>1010100</v>
       </c>
       <c r="H68" s="4" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="I68" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="J68" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="K68" s="4" t="s">
         <v>148</v>
       </c>
-      <c r="J68" s="4" t="s">
+      <c r="L68" s="4" t="s">
         <v>148</v>
-      </c>
-      <c r="K68" s="4" t="s">
-        <v>150</v>
-      </c>
-      <c r="L68" s="4" t="s">
-        <v>150</v>
       </c>
       <c r="M68" s="4">
         <v>31313131</v>
       </c>
       <c r="N68" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="69" spans="1:14" x14ac:dyDescent="0.2">
@@ -3794,34 +3835,34 @@
         <v>1</v>
       </c>
       <c r="E69" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="F69" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="G69" s="4">
         <v>1010100</v>
       </c>
       <c r="H69" s="4" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="I69" s="4" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="J69" s="4" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="K69" s="4" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="L69" s="4" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="M69" s="4">
         <v>31313131</v>
       </c>
       <c r="N69" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="70" spans="1:14" x14ac:dyDescent="0.2">
@@ -3838,34 +3879,34 @@
         <v>1</v>
       </c>
       <c r="E70" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="F70" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="G70" s="4">
         <v>1010100</v>
       </c>
       <c r="H70" s="4" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="I70" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="J70" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="K70" s="4" t="s">
         <v>154</v>
       </c>
-      <c r="J70" s="4" t="s">
-        <v>139</v>
-      </c>
-      <c r="K70" s="4" t="s">
-        <v>156</v>
-      </c>
       <c r="L70" s="4" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="M70" s="4">
         <v>32472623</v>
       </c>
       <c r="N70" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="71" spans="1:14" x14ac:dyDescent="0.2">
@@ -3882,28 +3923,28 @@
         <v>2</v>
       </c>
       <c r="E71" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="F71" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="G71" s="4">
         <v>1020100</v>
       </c>
       <c r="H71" s="4" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="I71" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="J71" s="4" t="s">
         <v>148</v>
       </c>
-      <c r="J71" s="4" t="s">
-        <v>150</v>
-      </c>
       <c r="K71" s="4">
         <v>0</v>
       </c>
       <c r="L71" s="4" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="M71" s="4"/>
     </row>
@@ -3921,28 +3962,28 @@
         <v>2</v>
       </c>
       <c r="E72" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="F72" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="G72" s="4">
         <v>1020100</v>
       </c>
       <c r="H72" s="4" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="I72" s="4" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="J72" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="K72" s="4">
+        <v>0</v>
+      </c>
+      <c r="L72" s="4" t="s">
         <v>154</v>
-      </c>
-      <c r="K72" s="4">
-        <v>0</v>
-      </c>
-      <c r="L72" s="4" t="s">
-        <v>156</v>
       </c>
       <c r="M72" s="4"/>
     </row>
@@ -3960,28 +4001,28 @@
         <v>1</v>
       </c>
       <c r="E73" t="s">
+        <v>91</v>
+      </c>
+      <c r="F73" t="s">
         <v>93</v>
-      </c>
-      <c r="F73" t="s">
-        <v>95</v>
       </c>
       <c r="G73" s="4">
         <v>1020100</v>
       </c>
       <c r="H73" s="4" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="I73" s="4" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="J73" s="4" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="K73" s="4">
         <v>0</v>
       </c>
       <c r="L73" s="4" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="M73" s="4"/>
     </row>
@@ -3999,28 +4040,28 @@
         <v>1</v>
       </c>
       <c r="E74" t="s">
+        <v>91</v>
+      </c>
+      <c r="F74" t="s">
         <v>93</v>
-      </c>
-      <c r="F74" t="s">
-        <v>95</v>
       </c>
       <c r="G74" s="4">
         <v>1020100</v>
       </c>
       <c r="H74" s="4" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="I74" s="4" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="J74" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="K74" s="4">
+        <v>0</v>
+      </c>
+      <c r="L74" s="4" t="s">
         <v>148</v>
-      </c>
-      <c r="K74" s="4">
-        <v>0</v>
-      </c>
-      <c r="L74" s="4" t="s">
-        <v>150</v>
       </c>
       <c r="M74" s="4"/>
     </row>
@@ -4038,34 +4079,34 @@
         <v>1</v>
       </c>
       <c r="E75" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="F75" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="G75" s="4">
         <v>1010100</v>
       </c>
       <c r="H75" s="4" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="I75" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="J75" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="K75" s="4" t="s">
         <v>156</v>
       </c>
-      <c r="J75" s="4" t="s">
+      <c r="L75" s="4" t="s">
         <v>148</v>
-      </c>
-      <c r="K75" s="4" t="s">
-        <v>158</v>
-      </c>
-      <c r="L75" s="4" t="s">
-        <v>150</v>
       </c>
       <c r="M75" s="4">
         <v>31313131</v>
       </c>
       <c r="N75" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="76" spans="1:14" x14ac:dyDescent="0.2">
@@ -4082,28 +4123,28 @@
         <v>2</v>
       </c>
       <c r="E76" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="F76" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="G76" s="4">
         <v>1020100</v>
       </c>
       <c r="H76" s="4" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="I76" s="4" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="J76" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="K76" s="4">
+        <v>0</v>
+      </c>
+      <c r="L76" s="4" t="s">
         <v>156</v>
-      </c>
-      <c r="K76" s="4">
-        <v>0</v>
-      </c>
-      <c r="L76" s="4" t="s">
-        <v>158</v>
       </c>
       <c r="M76" s="4"/>
     </row>
@@ -4121,34 +4162,34 @@
         <v>1</v>
       </c>
       <c r="E77" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="F77" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="G77" s="4">
         <v>1010100</v>
       </c>
       <c r="H77" s="4" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="I77" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="J77" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="K77" s="4" t="s">
         <v>158</v>
       </c>
-      <c r="J77" s="4" t="s">
+      <c r="L77" s="4" t="s">
         <v>148</v>
-      </c>
-      <c r="K77" s="4" t="s">
-        <v>160</v>
-      </c>
-      <c r="L77" s="4" t="s">
-        <v>150</v>
       </c>
       <c r="M77" s="4">
         <v>31313131</v>
       </c>
       <c r="N77" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="78" spans="1:14" x14ac:dyDescent="0.2">
@@ -4165,34 +4206,34 @@
         <v>1</v>
       </c>
       <c r="E78" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="F78" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="G78" s="4">
         <v>1010100</v>
       </c>
       <c r="H78" s="4" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="I78" s="4" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="J78" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="K78" s="4" t="s">
+        <v>159</v>
+      </c>
+      <c r="L78" s="4" t="s">
         <v>148</v>
       </c>
-      <c r="K78" s="4" t="s">
-        <v>161</v>
-      </c>
-      <c r="L78" s="4" t="s">
+      <c r="M78" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="N78" t="s">
         <v>150</v>
-      </c>
-      <c r="M78" s="4" t="s">
-        <v>151</v>
-      </c>
-      <c r="N78" t="s">
-        <v>152</v>
       </c>
     </row>
     <row r="79" spans="1:14" x14ac:dyDescent="0.2">
@@ -4209,34 +4250,34 @@
         <v>1</v>
       </c>
       <c r="E79" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="F79" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="G79" s="4">
         <v>1010100</v>
       </c>
       <c r="H79" s="4" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="I79" s="4" t="s">
+        <v>159</v>
+      </c>
+      <c r="J79" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="K79" s="4" t="s">
+        <v>160</v>
+      </c>
+      <c r="L79" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="M79" s="4" t="s">
         <v>161</v>
       </c>
-      <c r="J79" s="4" t="s">
-        <v>148</v>
-      </c>
-      <c r="K79" s="4" t="s">
+      <c r="N79" t="s">
         <v>162</v>
-      </c>
-      <c r="L79" s="4" t="s">
-        <v>150</v>
-      </c>
-      <c r="M79" s="4" t="s">
-        <v>163</v>
-      </c>
-      <c r="N79" t="s">
-        <v>164</v>
       </c>
     </row>
     <row r="80" spans="1:14" x14ac:dyDescent="0.2">
@@ -4253,28 +4294,28 @@
         <v>2</v>
       </c>
       <c r="E80" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="F80" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="G80" s="4">
         <v>1020100</v>
       </c>
       <c r="H80" s="4" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="I80" s="4" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="J80" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="K80" s="4">
+        <v>0</v>
+      </c>
+      <c r="L80" s="4" t="s">
         <v>158</v>
-      </c>
-      <c r="K80" s="4">
-        <v>0</v>
-      </c>
-      <c r="L80" s="4" t="s">
-        <v>160</v>
       </c>
       <c r="M80" s="4"/>
     </row>
@@ -4292,28 +4333,28 @@
         <v>2</v>
       </c>
       <c r="E81" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="F81" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="G81" s="4">
         <v>1020100</v>
       </c>
       <c r="H81" s="4" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="I81" s="4" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="J81" s="4" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="K81" s="4">
         <v>0</v>
       </c>
       <c r="L81" s="4" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="M81" s="4"/>
     </row>
@@ -4331,28 +4372,28 @@
         <v>2</v>
       </c>
       <c r="E82" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="F82" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="G82" s="4">
         <v>1020100</v>
       </c>
       <c r="H82" s="4" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="I82" s="4" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="J82" s="4" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="K82" s="4">
         <v>0</v>
       </c>
       <c r="L82" s="4" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="M82" s="4"/>
     </row>

</xml_diff>